<commit_message>
add checkin and notification intent, new notification.py and modified dialogflow_msg.py and users_database.py.
</commit_message>
<xml_diff>
--- a/WK's Folder/chatbot_app/components/database.xlsx
+++ b/WK's Folder/chatbot_app/components/database.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ISS-TYS\Documents\covid19-bot\WK's Folder\chatbot_app\components\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ISS-TYS\Documents\local_repo\covid19-bot\WK's Folder\chatbot_app\components\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BC7E8F4-0E58-44B1-909B-8DB034F5E1AA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85833933-C1F0-4E6A-BDD4-98C9545B203B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="570" yWindow="3165" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29655" yWindow="3255" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,27 +25,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Call for ambulance if your symptoms is getting worse and go to Emergency Department immediately at local hospital.</t>
   </si>
   <si>
-    <t>Please comply the instructions given by Quarantine Officer should you served Quarantine Order or issued a Stay Home Notice.</t>
-  </si>
-  <si>
-    <t>Please isolate yourself immediately and self-monitor. Ask me again should you develop any symptoms.</t>
-  </si>
-  <si>
-    <t>Please stay at home and self monitor for 2-3 days. If your symptom persist, consult doctor at GP.</t>
-  </si>
-  <si>
-    <t>Symptom could be caused by other conditions. Visit GP if needed and wear mask.</t>
-  </si>
-  <si>
     <t>You are in healthy condition. Self monitor for any new symptom.</t>
   </si>
   <si>
     <t>Responses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please stay at home and self monitor for 2-3 days. If your symptom persist, consult doctor at GP. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please comply the instructions given by Quarantine Officer should you served Quarantine Order or issued a Stay Home Notice. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Symptom could be caused by other conditions. Visit GP if needed and wear mask. </t>
+  </si>
+  <si>
+    <t>QueryID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please isolate yourself immediately and self-monitor should you develop any symptoms. </t>
   </si>
 </sst>
 </file>
@@ -371,50 +374,72 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="133.42578125" customWidth="1"/>
+    <col min="1" max="1" width="156.5703125" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update from tyseng on notification + multip + feedback_text
</commit_message>
<xml_diff>
--- a/WK's Folder/chatbot_app/components/database.xlsx
+++ b/WK's Folder/chatbot_app/components/database.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ISS-TYS\Documents\covid19-bot\WK's Folder\chatbot_app\components\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ISS-TYS\Documents\local_repo\covid19-bot\WK's Folder\chatbot_app\components\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BC7E8F4-0E58-44B1-909B-8DB034F5E1AA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85833933-C1F0-4E6A-BDD4-98C9545B203B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="570" yWindow="3165" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29655" yWindow="3255" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,27 +25,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Call for ambulance if your symptoms is getting worse and go to Emergency Department immediately at local hospital.</t>
   </si>
   <si>
-    <t>Please comply the instructions given by Quarantine Officer should you served Quarantine Order or issued a Stay Home Notice.</t>
-  </si>
-  <si>
-    <t>Please isolate yourself immediately and self-monitor. Ask me again should you develop any symptoms.</t>
-  </si>
-  <si>
-    <t>Please stay at home and self monitor for 2-3 days. If your symptom persist, consult doctor at GP.</t>
-  </si>
-  <si>
-    <t>Symptom could be caused by other conditions. Visit GP if needed and wear mask.</t>
-  </si>
-  <si>
     <t>You are in healthy condition. Self monitor for any new symptom.</t>
   </si>
   <si>
     <t>Responses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please stay at home and self monitor for 2-3 days. If your symptom persist, consult doctor at GP. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please comply the instructions given by Quarantine Officer should you served Quarantine Order or issued a Stay Home Notice. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Symptom could be caused by other conditions. Visit GP if needed and wear mask. </t>
+  </si>
+  <si>
+    <t>QueryID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please isolate yourself immediately and self-monitor should you develop any symptoms. </t>
   </si>
 </sst>
 </file>
@@ -371,50 +374,72 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="133.42578125" customWidth="1"/>
+    <col min="1" max="1" width="156.5703125" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "add checkin and notification intent, new notification.py and modified dialogflow_msg.py and users_database.py."
This reverts commit 0f239c174eee83f0d502b9b5420bd8dac05c2571.
</commit_message>
<xml_diff>
--- a/WK's Folder/chatbot_app/components/database.xlsx
+++ b/WK's Folder/chatbot_app/components/database.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ISS-TYS\Documents\local_repo\covid19-bot\WK's Folder\chatbot_app\components\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ISS-TYS\Documents\covid19-bot\WK's Folder\chatbot_app\components\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85833933-C1F0-4E6A-BDD4-98C9545B203B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BC7E8F4-0E58-44B1-909B-8DB034F5E1AA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29655" yWindow="3255" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="570" yWindow="3165" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,30 +25,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Call for ambulance if your symptoms is getting worse and go to Emergency Department immediately at local hospital.</t>
   </si>
   <si>
+    <t>Please comply the instructions given by Quarantine Officer should you served Quarantine Order or issued a Stay Home Notice.</t>
+  </si>
+  <si>
+    <t>Please isolate yourself immediately and self-monitor. Ask me again should you develop any symptoms.</t>
+  </si>
+  <si>
+    <t>Please stay at home and self monitor for 2-3 days. If your symptom persist, consult doctor at GP.</t>
+  </si>
+  <si>
+    <t>Symptom could be caused by other conditions. Visit GP if needed and wear mask.</t>
+  </si>
+  <si>
     <t>You are in healthy condition. Self monitor for any new symptom.</t>
   </si>
   <si>
     <t>Responses</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Please stay at home and self monitor for 2-3 days. If your symptom persist, consult doctor at GP. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Please comply the instructions given by Quarantine Officer should you served Quarantine Order or issued a Stay Home Notice. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Symptom could be caused by other conditions. Visit GP if needed and wear mask. </t>
-  </si>
-  <si>
-    <t>QueryID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Please isolate yourself immediately and self-monitor should you develop any symptoms. </t>
   </si>
 </sst>
 </file>
@@ -374,72 +371,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="156.5703125" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="133.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>5</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>